<commit_message>
Add examples and finalization function post data
</commit_message>
<xml_diff>
--- a/api/data_api_test.xlsx
+++ b/api/data_api_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\E0443815\projet_tec\stage3A\api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB45662-1347-429F-9CEB-9A512A3F61B5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7480340-780C-47FC-BD9B-F8F5A71C6943}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,67 +25,85 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
-  <si>
-    <t>168.124.108.137</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t>tcp/135</t>
+  </si>
+  <si>
+    <t>1060</t>
+  </si>
+  <si>
+    <t>IP SRC</t>
+  </si>
+  <si>
+    <t>IP DST</t>
+  </si>
+  <si>
+    <t>PORT DST</t>
+  </si>
+  <si>
+    <t>COUNT</t>
+  </si>
+  <si>
+    <t>1061</t>
   </si>
   <si>
     <t>tcp/135,54670</t>
   </si>
   <si>
-    <t>1350</t>
-  </si>
-  <si>
-    <t>157.206.121.198</t>
-  </si>
-  <si>
-    <t>168.124.108.19</t>
-  </si>
-  <si>
-    <t>tcp/135</t>
-  </si>
-  <si>
-    <t>1060</t>
-  </si>
-  <si>
-    <t>tcp/&gt;49151</t>
-  </si>
-  <si>
-    <t>1057</t>
-  </si>
-  <si>
-    <t>7.37.145.157,7.28.153.55,7.28.147.91,7.28.84.141,7.28.145.191,7.28.83.198,7.28.157.108</t>
-  </si>
-  <si>
-    <t>611</t>
-  </si>
-  <si>
-    <t>IP SRC</t>
-  </si>
-  <si>
-    <t>IP DST</t>
-  </si>
-  <si>
-    <t>PORT DST</t>
-  </si>
-  <si>
-    <t>COUNT</t>
-  </si>
-  <si>
-    <t>168.124.12.128/25,7.28.159.205</t>
-  </si>
-  <si>
-    <t>168.124.108.19,168.124.108.20</t>
-  </si>
-  <si>
-    <t>tcp/22;udp/55834</t>
+    <t>168.124.108.0/24</t>
+  </si>
+  <si>
+    <t>udp/111</t>
+  </si>
+  <si>
+    <t>tcp/15000</t>
+  </si>
+  <si>
+    <t>1063</t>
+  </si>
+  <si>
+    <t>1064</t>
+  </si>
+  <si>
+    <t>1065</t>
+  </si>
+  <si>
+    <t>10.0.0.1</t>
+  </si>
+  <si>
+    <t>168.124.198.237,10.0.0.2</t>
+  </si>
+  <si>
+    <t>tcp/61241-62000</t>
+  </si>
+  <si>
+    <t>10.0.0.2</t>
+  </si>
+  <si>
+    <t>192.168.1.1</t>
+  </si>
+  <si>
+    <t>192.168.1.7</t>
+  </si>
+  <si>
+    <t>10.12.0.2</t>
+  </si>
+  <si>
+    <t>10.0.0.2,10.0.0.9,10.0.0.98,10.0.1.2</t>
+  </si>
+  <si>
+    <t>192.168.1.0/26</t>
+  </si>
+  <si>
+    <t>168.124.100.143</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,6 +115,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -408,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -423,41 +447,41 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
@@ -465,33 +489,48 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="1" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>